<commit_message>
Excel formatter works; CPSC 4000 is scheduled incorrectly.
</commit_message>
<xml_diff>
--- a/src/input_files/Path To Graduation Y.xlsx
+++ b/src/input_files/Path To Graduation Y.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mel91\Desktop\lew\scheduler\src\input_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mel91\Desktop\lew8\scheduler\src\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC3A1FA-BABB-40D5-ACA7-79CD6BA8EF83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56CE5C39-9A27-4723-8F31-D39D76764C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="36">
   <si>
     <t>Path to Graduation</t>
   </si>
@@ -98,58 +98,13 @@
     <t>CPSC 4176 - Senior Software Eng. Project (-- Sp --)</t>
   </si>
   <si>
-    <t>Fall 2022</t>
-  </si>
-  <si>
-    <t>Spring 2023</t>
-  </si>
-  <si>
-    <t>Summer 2023</t>
-  </si>
-  <si>
     <t>CPSC 4000 - Baccalaureate Survey (Fa Sp Su)</t>
   </si>
   <si>
     <t>Take during your last semester</t>
   </si>
   <si>
-    <t>Fall 2023</t>
-  </si>
-  <si>
-    <t>Spring 2024</t>
-  </si>
-  <si>
-    <t>Summer 2024</t>
-  </si>
-  <si>
     <t>Total Credit Hours</t>
-  </si>
-  <si>
-    <t>Fall 2024</t>
-  </si>
-  <si>
-    <t>Spring 2025</t>
-  </si>
-  <si>
-    <t>Summer 2025</t>
-  </si>
-  <si>
-    <t>Fall 2025</t>
-  </si>
-  <si>
-    <t>Spring 2026</t>
-  </si>
-  <si>
-    <t>Summer 2026</t>
-  </si>
-  <si>
-    <t>Fall 2026</t>
-  </si>
-  <si>
-    <t>Spring 2027</t>
-  </si>
-  <si>
-    <t>Summer 2027</t>
   </si>
   <si>
     <r>
@@ -231,6 +186,15 @@
   </si>
   <si>
     <t>CPSC 4157 - Computer Networks (Fa -- Su)</t>
+  </si>
+  <si>
+    <t>Fall 20__</t>
+  </si>
+  <si>
+    <t>Spring 20__</t>
+  </si>
+  <si>
+    <t>Summer 20__</t>
   </si>
 </sst>
 </file>
@@ -593,31 +557,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="52">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="17" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -625,29 +587,24 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="17" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="17" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="17" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="17" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="17" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -655,13 +612,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="17" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -990,7 +946,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:J26"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1010,24 +966,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="55"/>
-      <c r="B1" s="56"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="56"/>
+      <c r="A1" s="49"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:26" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="1">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
       <c r="H2" s="3" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>1</v>
@@ -1038,30 +994,29 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="58" t="s">
+      <c r="H3" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="58">
+      <c r="I3" s="48">
         <v>4</v>
       </c>
-      <c r="J3" s="59"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
@@ -1070,13 +1025,12 @@
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
-      <c r="H4" s="58" t="s">
-        <v>40</v>
-      </c>
-      <c r="I4" s="58">
+      <c r="H4" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="48">
         <v>4</v>
       </c>
-      <c r="J4" s="59"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
@@ -1085,13 +1039,12 @@
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
-      <c r="H5" s="58" t="s">
+      <c r="H5" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="58">
+      <c r="I5" s="48">
         <v>3</v>
       </c>
-      <c r="J5" s="59"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11"/>
@@ -1100,122 +1053,118 @@
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
       <c r="F6" s="11"/>
-      <c r="H6" s="58" t="s">
-        <v>41</v>
-      </c>
-      <c r="I6" s="58">
+      <c r="H6" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="48">
         <v>3</v>
       </c>
-      <c r="J6" s="59"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
       <c r="E7" s="11"/>
       <c r="F7" s="11"/>
-      <c r="H7" s="58" t="s">
-        <v>42</v>
-      </c>
-      <c r="I7" s="58">
+      <c r="H7" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="48">
         <v>3</v>
       </c>
-      <c r="J7" s="59"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="11"/>
-      <c r="H8" s="58" t="s">
+      <c r="H8" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="58">
+      <c r="I8" s="48">
         <v>3</v>
       </c>
-      <c r="J8" s="58" t="s">
+      <c r="J8" s="48" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
       <c r="E9" s="11"/>
       <c r="F9" s="11"/>
-      <c r="H9" s="58" t="s">
+      <c r="H9" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="58">
+      <c r="I9" s="48">
         <v>3</v>
       </c>
-      <c r="J9" s="59"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="14">
         <f>SUM(B4:B9)</f>
         <v>0</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="14">
         <f>SUM(D4:D9)</f>
         <v>0</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="14">
         <f>SUM(F4:F9)</f>
         <v>0</v>
       </c>
-      <c r="H10" s="58" t="s">
+      <c r="H10" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="58">
+      <c r="I10" s="48">
         <v>3</v>
       </c>
-      <c r="J10" s="59"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="17" t="s">
+      <c r="A11" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="19" t="s">
+      <c r="C11" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="21" t="s">
+      <c r="E11" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="G11" s="22"/>
-      <c r="H11" s="59" t="s">
+      <c r="G11" s="20"/>
+      <c r="H11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="58">
+      <c r="I11" s="48">
         <v>3</v>
       </c>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="22"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
@@ -1232,17 +1181,16 @@
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
-      <c r="C12" s="23"/>
+      <c r="C12" s="21"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
-      <c r="H12" s="58" t="s">
+      <c r="H12" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="I12" s="58">
+      <c r="I12" s="48">
         <v>3</v>
       </c>
-      <c r="J12" s="59"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
@@ -1251,132 +1199,126 @@
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
-      <c r="H13" s="58" t="s">
+      <c r="H13" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="58">
+      <c r="I13" s="48">
         <v>3</v>
       </c>
-      <c r="J13" s="24" t="s">
+      <c r="J13" s="22" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="25"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="11"/>
-      <c r="C14" s="25"/>
+      <c r="C14" s="23"/>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
-      <c r="H14" s="58" t="s">
+      <c r="H14" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="58">
+      <c r="I14" s="48">
         <v>3</v>
       </c>
-      <c r="J14" s="59"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="25"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="11"/>
       <c r="C15" s="12"/>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
-      <c r="H15" s="58" t="s">
+      <c r="H15" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="58">
+      <c r="I15" s="48">
         <v>3</v>
       </c>
-      <c r="J15" s="59"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
-      <c r="H16" s="58" t="s">
+      <c r="H16" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="I16" s="58">
+      <c r="I16" s="48">
         <v>3</v>
       </c>
-      <c r="J16" s="59"/>
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
-      <c r="H17" s="58" t="s">
+      <c r="H17" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="I17" s="58">
+      <c r="I17" s="48">
         <v>3</v>
       </c>
-      <c r="J17" s="59"/>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="15">
+      <c r="B18" s="14">
         <f>SUM(B12:B17)</f>
         <v>0</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="14">
         <f>SUM(D12:D17)</f>
         <v>0</v>
       </c>
-      <c r="E18" s="26" t="s">
+      <c r="E18" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="15">
+      <c r="F18" s="14">
         <f>SUM(F12:F17)</f>
         <v>0</v>
       </c>
-      <c r="H18" s="58" t="s">
+      <c r="H18" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="I18" s="58">
+      <c r="I18" s="48">
         <v>3</v>
       </c>
-      <c r="J18" s="59"/>
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="28" t="s">
+      <c r="A19" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="30" t="s">
+      <c r="C19" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="E19" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="F19" s="32" t="s">
+      <c r="E19" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H19" s="58" t="s">
+      <c r="H19" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="I19" s="58">
+      <c r="I19" s="48">
         <v>3</v>
       </c>
-      <c r="J19" s="59"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10"/>
@@ -1385,18 +1327,18 @@
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="59" t="s">
+      <c r="G20" s="20"/>
+      <c r="H20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I20" s="58">
+      <c r="I20" s="48">
         <v>3</v>
       </c>
-      <c r="J20" s="22"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="22"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="22"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="20"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
@@ -1417,18 +1359,18 @@
       <c r="D21" s="11"/>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="59" t="s">
-        <v>43</v>
-      </c>
-      <c r="I21" s="58">
+      <c r="G21" s="20"/>
+      <c r="H21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I21" s="48">
         <v>3</v>
       </c>
-      <c r="J21" s="22"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="22"/>
-      <c r="M21" s="22"/>
-      <c r="N21" s="22"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="20"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
@@ -1448,13 +1390,12 @@
       <c r="D22" s="11"/>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
-      <c r="H22" s="58" t="s">
-        <v>44</v>
-      </c>
-      <c r="I22" s="58">
+      <c r="H22" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I22" s="48">
         <v>3</v>
       </c>
-      <c r="J22" s="59"/>
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="11"/>
@@ -1463,93 +1404,90 @@
       <c r="D23" s="11"/>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
-      <c r="H23" s="58" t="s">
-        <v>45</v>
-      </c>
-      <c r="I23" s="58">
+      <c r="H23" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="I23" s="48">
         <v>3</v>
       </c>
-      <c r="J23" s="59"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11"/>
-      <c r="B24" s="13"/>
+      <c r="B24" s="11"/>
       <c r="C24" s="11"/>
-      <c r="D24" s="13"/>
+      <c r="D24" s="11"/>
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
-      <c r="H24" s="58" t="s">
-        <v>46</v>
-      </c>
-      <c r="I24" s="58">
+      <c r="H24" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="I24" s="48">
         <v>3</v>
       </c>
-      <c r="J24" s="59"/>
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="11"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
-      <c r="H25" s="58" t="s">
-        <v>47</v>
-      </c>
-      <c r="I25" s="58">
+      <c r="H25" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="I25" s="48">
         <v>3</v>
       </c>
-      <c r="J25" s="59"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="33" t="s">
+      <c r="A26" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="34">
+      <c r="B26" s="31">
         <f>SUM(B20:B25)</f>
         <v>0</v>
       </c>
-      <c r="C26" s="35" t="s">
+      <c r="C26" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="D26" s="34">
+      <c r="D26" s="31">
         <f>SUM(D20:D25)</f>
         <v>0</v>
       </c>
-      <c r="E26" s="36" t="s">
+      <c r="E26" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="F26" s="15">
+      <c r="F26" s="14">
         <f>SUM(F20:F25)</f>
         <v>0</v>
       </c>
-      <c r="H26" s="58" t="s">
-        <v>24</v>
-      </c>
-      <c r="I26" s="58">
+      <c r="H26" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="I26" s="48">
         <v>0</v>
       </c>
-      <c r="J26" s="24" t="s">
-        <v>25</v>
+      <c r="J26" s="22" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="38" t="s">
+      <c r="B27" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="39" t="s">
+      <c r="C27" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="D27" s="40" t="s">
+      <c r="D27" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="E27" s="41" t="s">
+      <c r="E27" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F27" s="42" t="s">
+      <c r="F27" s="37" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1568,14 +1506,14 @@
       <c r="D29" s="11"/>
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="22"/>
-      <c r="J29" s="22"/>
-      <c r="K29" s="22"/>
-      <c r="L29" s="22"/>
-      <c r="M29" s="22"/>
-      <c r="N29" s="22"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="20"/>
+      <c r="L29" s="20"/>
+      <c r="M29" s="20"/>
+      <c r="N29" s="20"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
@@ -1596,14 +1534,14 @@
       <c r="D30" s="11"/>
       <c r="E30" s="11"/>
       <c r="F30" s="11"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="22"/>
-      <c r="J30" s="22"/>
-      <c r="K30" s="22"/>
-      <c r="L30" s="22"/>
-      <c r="M30" s="22"/>
-      <c r="N30" s="22"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="20"/>
+      <c r="L30" s="20"/>
+      <c r="M30" s="20"/>
+      <c r="N30" s="20"/>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
@@ -1627,94 +1565,94 @@
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11"/>
-      <c r="B32" s="13"/>
+      <c r="B32" s="11"/>
       <c r="C32" s="11"/>
-      <c r="D32" s="13"/>
+      <c r="D32" s="11"/>
       <c r="E32" s="11"/>
       <c r="F32" s="11"/>
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="11"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="33" t="s">
+      <c r="A34" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="34">
+      <c r="B34" s="31">
         <f>SUM(B28:B33)</f>
         <v>0</v>
       </c>
-      <c r="C34" s="35" t="s">
+      <c r="C34" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="D34" s="34">
+      <c r="D34" s="31">
         <f>SUM(D28:D33)</f>
         <v>0</v>
       </c>
-      <c r="E34" s="36" t="s">
+      <c r="E34" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="F34" s="15">
+      <c r="F34" s="14">
         <f>SUM(F28:F33)</f>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="43" t="s">
-        <v>36</v>
-      </c>
-      <c r="B35" s="44" t="s">
+      <c r="A35" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C35" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="D35" s="46" t="s">
+      <c r="C35" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="E35" s="47" t="s">
-        <v>38</v>
-      </c>
-      <c r="F35" s="48" t="s">
+      <c r="E35" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="F35" s="42" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
       <c r="B36" s="10"/>
-      <c r="C36" s="49"/>
-      <c r="D36" s="49"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="11"/>
       <c r="B37" s="11"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="13"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
+      <c r="A38" s="11"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
       <c r="E38" s="11"/>
       <c r="F38" s="11"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="22"/>
-      <c r="I38" s="22"/>
-      <c r="J38" s="22"/>
-      <c r="K38" s="22"/>
-      <c r="L38" s="22"/>
-      <c r="M38" s="22"/>
-      <c r="N38" s="22"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="20"/>
+      <c r="L38" s="20"/>
+      <c r="M38" s="20"/>
+      <c r="N38" s="20"/>
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
@@ -1729,57 +1667,57 @@
       <c r="Z38" s="1"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="13"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
       <c r="E39" s="11"/>
       <c r="F39" s="11"/>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="13"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
+      <c r="A40" s="11"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
       <c r="E40" s="11"/>
       <c r="F40" s="11"/>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="13"/>
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
+      <c r="A41" s="11"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
       <c r="E41" s="11"/>
       <c r="F41" s="11"/>
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="50" t="s">
+      <c r="A42" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="B42" s="51">
+      <c r="B42" s="44">
         <f>SUM(B36:B41)</f>
         <v>0</v>
       </c>
-      <c r="C42" s="50" t="s">
+      <c r="C42" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="D42" s="51">
+      <c r="D42" s="44">
         <f>SUM(D36:D41)</f>
         <v>0</v>
       </c>
-      <c r="E42" s="50" t="s">
+      <c r="E42" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="F42" s="52">
+      <c r="F42" s="45">
         <f>SUM(F35:F41)</f>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E43" s="53" t="s">
-        <v>29</v>
-      </c>
-      <c r="F43" s="54">
+      <c r="E43" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="F43" s="47">
         <f>SUM(B10+D10+F10+B18+D18+F18+B26+D26+F26+B34+D34+F34+B42+D42+F42)</f>
         <v>0</v>
       </c>

</xml_diff>